<commit_message>
Add Dropbox collection of questions
</commit_message>
<xml_diff>
--- a/company/dropbox/question.xlsx
+++ b/company/dropbox/question.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bozhou/Work/interview/company/dropbox/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D4CBD766-0F6D-324B-8FCF-A00A93035867}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CBA3C3E-0533-8349-9B67-10BDFD60C79D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="50260" yWindow="3400" windowWidth="20020" windowHeight="16120" xr2:uid="{FF1F46D0-5BD5-4042-B7C2-080A419A491A}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="52">
   <si>
     <t>LC 609</t>
   </si>
@@ -63,9 +63,6 @@
     <t>Game of life</t>
   </si>
   <si>
-    <t>NASA 存图片?</t>
-  </si>
-  <si>
     <t xml:space="preserve"> https://www.1point3acres.com/bbs/thread-529802-1-1.html</t>
   </si>
   <si>
@@ -78,31 +75,150 @@
     <t>https://www.1point3acres.com/bbs/thread-529186-1-1.html</t>
   </si>
   <si>
-    <t>https://www.1point3acres.com/bbs/thread-531705-1-1.html https://www.1point3acres.com/bbs/thread-528854-1-1.html</t>
-  </si>
-  <si>
     <t>web crawler，直接多线程版</t>
   </si>
   <si>
     <t>id generator，各种解法，详细解释了bitset的做法</t>
+  </si>
+  <si>
+    <t>given file path name, and a buffer, ==&gt; find if the file contains the buffer
+boolean contains(String filePath, byte[] buffer){ }
+filePath "a.txt" == "abba"
+contains("a.txt", "ab") --&gt; true
+contains("a.txt", "bb") --&gt; true
+contains("a.txt", "cb") --&gt; false</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+https://www.1point3acres.com/bbs/thread-528831-1-1.html</t>
+  </si>
+  <si>
+    <t>给了一个section(int x, int y) 和Image class， 求storeImage(section, Image) 和 Image fetch(section). follow up 是 section getstalest(section);</t>
+  </si>
+  <si>
+    <t>https://www.1point3acres.com/bbs/thread-526980-1-1.html</t>
+  </si>
+  <si>
+    <t>https://www.1point3acres.com/bbs/thread-526776-1-1.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.1point3acres.com/bbs/thread-531705-1-1.html </t>
+  </si>
+  <si>
+    <t>https://www.1point3acres.com/bbs/thread-528854-1-1.html</t>
+  </si>
+  <si>
+    <t>用户发request是一个image的url，让design一个系统process这个request并发给consumer，不同consumer接收，然后处理，变成thumbnail存在db。</t>
+  </si>
+  <si>
+    <t>https://www.1point3acres.com/bbs/thread-525005-1-1.html</t>
+  </si>
+  <si>
+    <t>token buckets + multi-thread。基本解法就很快写完了，然后要加锁</t>
+  </si>
+  <si>
+    <t>log system</t>
+  </si>
+  <si>
+    <t>design a log system that allow application to record server events such as hardware replacement / request response error. Data can then be used offline and online for analysis.</t>
+  </si>
+  <si>
+    <t>https://www.1point3acres.com/bbs/thread-524141-1-1.html</t>
+  </si>
+  <si>
+    <t>implement an ID generator that supports 2 methods: alloc() and release(id), alloc() ID from 0 to MAX. how much memory is needed for each solution? what are the runtimes? how to optimize and make tradeoff between runtime and space.</t>
+  </si>
+  <si>
+    <t>implement a web crawler and then make it multi-threaded and thread-safe</t>
+  </si>
+  <si>
+    <t>https://www.1point3acres.com/bbs/thread-523051-1-1.html</t>
+  </si>
+  <si>
+    <t>database atomic transaction design，实现几个methods:
+read(txid, key)
+write(txid, key, value)
+createTransaction()
+commit(txid)
+其中有几个关键:
+1. 要支持roll back. 
+2. 一个txid不能写同一个key到别的txid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">给你一堆卫星图片表示星空某个地方的坐标XY 存储图片 你给nasa做这个东西管理 怎么设计存储。 正解是写个lru cache </t>
+  </si>
+  <si>
+    <t>https://www.1point3acres.com/bbs/thread-511212-1-1.html</t>
+  </si>
+  <si>
+    <t>要求设计一个数据结构保存1000x1000个1Mb的图片，按矩阵排列，完成init(row, col), update(row, col, image), get(row, col)
+1. 用二位数组完成
+2. follow up，解决内存的问题， 因为用数组保存，普通计算机的内存肯定不够用
+3. follow up, 要一个getStale() 的函数，得到所有图片中最老的图片的[row, col]坐标</t>
+  </si>
+  <si>
+    <t>https://www.1point3acres.com/bbs/thread-519415-1-1.html</t>
+  </si>
+  <si>
+    <t>https://www.1point3acres.com/bbs/thread-518593-1-1.html</t>
+  </si>
+  <si>
+    <t>design dropbox, 问的非常细， 前台后台， 如何sync 不同的client， version化</t>
+  </si>
+  <si>
+    <t>让你写一个API，可以传进去一个function和一个时间，然后这个function会被延迟这么多时间被执行。 这个API可以被反复call， 相当于可以schedule不止一个要被延迟处理的function。</t>
+  </si>
+  <si>
+    <t>https://www.1point3acres.com/bbs/thread-517752-1-1.html</t>
+  </si>
+  <si>
+    <t>https://www.1point3acres.com/bbs/thread-517218-1-1.html</t>
+  </si>
+  <si>
+    <t>假设星空是一个二维空间，空间分成M*N个区域 （0&lt;= M, N&lt;=1000). 
+NASA平时会对一个区域 (i，j) 照相，每张照片大小是 1-2M，，然后存起来，平时也会来取照片，实现两个方法
+Class Imaige{}
+void storeImage （Imaige i，int i，int j）
+Image loadImaige （int i，int j）
+之后实现下面的方法，这个方法会返回，更新时间最早的区域（i，j），如果更新时间相同，返回任意一个区域，如果有没被更新的区域，返回其中任何一个区域
+int[] findOldestImage()</t>
+  </si>
+  <si>
+    <t>delay setTimeout</t>
+  </si>
+  <si>
+    <t>https://www.1point3acres.com/bbs/thread-514986-1-1.html</t>
+  </si>
+  <si>
+    <t>https://www.1point3acres.com/bbs/thread-510124-1-1.html</t>
+  </si>
+  <si>
+    <t>https://www.1point3acres.com/bbs/thread-509723-1-1.html</t>
+  </si>
+  <si>
+    <t>merge/delete intervals, 如果delete连续的intervals，怎么做比较好</t>
+  </si>
+  <si>
+    <t>design ring buffer</t>
+  </si>
+  <si>
+    <t>implement read/write lock, 当多读少写，如何优化</t>
+  </si>
+  <si>
+    <t>https://www.1point3acres.com/bbs/thread-505809-1-1.html</t>
+  </si>
+  <si>
+    <t>phone number dictionary</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -125,16 +241,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -447,15 +564,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2C395D0-B9AD-E54D-9D2D-3754DE058F1F}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26" customWidth="1"/>
+    <col min="1" max="1" width="57.33203125" customWidth="1"/>
     <col min="2" max="2" width="75.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -474,73 +591,58 @@
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>14</v>
+      <c r="B2" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="C2">
-        <v>5</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
+      <c r="B3" s="2" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
+      <c r="B4" s="2" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
+      <c r="B6" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="C7">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8">
-        <v>2</v>
+      <c r="B8" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -548,7 +650,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -556,23 +658,236 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B13" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B14" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="136" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="C19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B21" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="136" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="119" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="187" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>39</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>51</v>
+      </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" xr:uid="{7E913D06-2438-EF45-AC05-B1530CAF0127}"/>
-    <hyperlink ref="B4" r:id="rId2" display="https://www.1point3acres.com/bbs/thread-531705-1-1.html" xr:uid="{1D98C08E-F190-744F-B73C-B5EC6E3842F2}"/>
-    <hyperlink ref="B2" r:id="rId3" xr:uid="{1C4A6E72-11C6-4644-A666-2E64E184F678}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adding more source code
</commit_message>
<xml_diff>
--- a/company/dropbox/question.xlsx
+++ b/company/dropbox/question.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bozhou/Dropbox/interview/company/dropbox/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF6E8A17-D4E0-7642-A803-C9A738B3506A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A764AC1-1D66-7F48-A4DF-D178855E8C69}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7800" yWindow="460" windowWidth="17800" windowHeight="14180" xr2:uid="{FF1F46D0-5BD5-4042-B7C2-080A419A491A}"/>
+    <workbookView xWindow="45780" yWindow="5080" windowWidth="17800" windowHeight="14180" xr2:uid="{FF1F46D0-5BD5-4042-B7C2-080A419A491A}"/>
   </bookViews>
   <sheets>
     <sheet name="freq" sheetId="2" r:id="rId1"/>
@@ -720,7 +720,7 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Add a LOT questions
</commit_message>
<xml_diff>
--- a/company/dropbox/question.xlsx
+++ b/company/dropbox/question.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bozhou/Dropbox/interview/company/dropbox/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06947767-8411-1748-98FE-6E23FCB48F23}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51671EB1-D1A1-5A46-8D64-B1B0D251E381}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="72440" yWindow="6900" windowWidth="17800" windowHeight="14180" xr2:uid="{FF1F46D0-5BD5-4042-B7C2-080A419A491A}"/>
+    <workbookView xWindow="9300" yWindow="1080" windowWidth="16300" windowHeight="13180" xr2:uid="{FF1F46D0-5BD5-4042-B7C2-080A419A491A}"/>
   </bookViews>
   <sheets>
     <sheet name="freq" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="105">
   <si>
     <t>LC 609</t>
   </si>
@@ -349,12 +349,36 @@
   <si>
     <t>https://www.1point3acres.com/bbs/thread-544660-1-1.html</t>
   </si>
+  <si>
+    <t>https://www.1point3acres.com/bbs/thread-545571-1-1.html</t>
+  </si>
+  <si>
+    <t>https://bravenewgeek.com/building-a-distributed-log-from-scratch-part-1-storage-mechanics/</t>
+  </si>
+  <si>
+    <t>https://dzone.com/articles/distributed-logging-architecture-for-microservices</t>
+  </si>
+  <si>
+    <t>https://blog.csdn.net/siddontang/article/details/8958323</t>
+  </si>
+  <si>
+    <t>https://www.cnblogs.com/wangtao_20/p/3481098.html</t>
+  </si>
+  <si>
+    <t>https://www.cnblogs.com/davidwang456/articles/8360274.html</t>
+  </si>
+  <si>
+    <t>设计message queue的读取的API</t>
+  </si>
+  <si>
+    <t>https://www.1point3acres.com/bbs/thread-546698-1-1.html</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -373,6 +397,29 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -399,7 +446,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -408,6 +455,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -726,7 +776,7 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -784,23 +834,26 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="D4">
-        <v>9</v>
-      </c>
-      <c r="E4" s="5" t="s">
+      <c r="D4" s="6">
+        <v>10</v>
+      </c>
+      <c r="E4" s="7" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="D5">
-        <v>12</v>
+      <c r="B5" s="6">
+        <v>379</v>
+      </c>
+      <c r="D5" s="6">
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -883,17 +936,17 @@
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="13" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="3">
         <v>3</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F13" s="8" t="s">
         <v>94</v>
       </c>
     </row>
@@ -905,17 +958,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+    <row r="15" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="3">
         <v>4</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="E15" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="F15" s="8" t="s">
         <v>31</v>
       </c>
     </row>
@@ -927,14 +980,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+    <row r="17" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="3">
         <v>4</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="E17" s="8" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1015,10 +1068,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{473A6A2A-39F5-B04D-84D8-530F090E5F3A}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1026,7 +1079,7 @@
     <col min="1" max="1" width="66.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>61</v>
       </c>
@@ -1034,116 +1087,152 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>52</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="68" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>72</v>
       </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>76</v>
       </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="B7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B7">
+      <c r="B8" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="C8" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>79</v>
       </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="B9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>80</v>
       </c>
-      <c r="B9">
+      <c r="B10">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>48</v>
       </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="B11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>86</v>
       </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="B12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>88</v>
       </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12" s="5" t="s">
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>90</v>
       </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="B14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B14">
-        <v>1</v>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C12" r:id="rId1" xr:uid="{BC489624-21F6-954B-8329-5EAB6161A1FE}"/>
+    <hyperlink ref="C13" r:id="rId1" xr:uid="{BC489624-21F6-954B-8329-5EAB6161A1FE}"/>
+    <hyperlink ref="C15" r:id="rId2" xr:uid="{5B25B5A1-3FAF-6348-86BE-CA72D64F5B41}"/>
+    <hyperlink ref="C8" r:id="rId3" xr:uid="{B8628CF6-74AF-9A48-87FD-E099FBD36136}"/>
+    <hyperlink ref="D8" r:id="rId4" xr:uid="{DAA6E1F5-830D-B043-8D78-8FAD82A11247}"/>
+    <hyperlink ref="C5" r:id="rId5" xr:uid="{7662A22F-9DAF-7A4C-BA3B-68C2EC8002A9}"/>
+    <hyperlink ref="D5" r:id="rId6" xr:uid="{15A83721-4991-A041-B1C1-ECAA40FDFF81}"/>
+    <hyperlink ref="E8" r:id="rId7" xr:uid="{0718B7A4-7742-DF4C-B52C-F4A83410E99E}"/>
+    <hyperlink ref="C2" r:id="rId8" xr:uid="{24D4A1BB-57A6-2B4D-B0DE-7111546A162F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>